<commit_message>
connected robotrainer and program creator
</commit_message>
<xml_diff>
--- a/moeed.xlsx
+++ b/moeed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>WEEK 1</t>
   </si>
@@ -25,46 +25,61 @@
     <t>Cable Flies</t>
   </si>
   <si>
+    <t>4x6</t>
+  </si>
+  <si>
+    <t>DB Press</t>
+  </si>
+  <si>
+    <t>3x12</t>
+  </si>
+  <si>
+    <t>Incline DB Press</t>
+  </si>
+  <si>
     <t>3x10</t>
   </si>
   <si>
-    <t>DB Press</t>
+    <t>Incline Press Machine</t>
+  </si>
+  <si>
+    <t>4x8</t>
+  </si>
+  <si>
+    <t>DAY 2</t>
+  </si>
+  <si>
+    <t>4x10</t>
+  </si>
+  <si>
+    <t>3x6</t>
+  </si>
+  <si>
+    <t>DAY 3</t>
+  </si>
+  <si>
+    <t>4x12</t>
+  </si>
+  <si>
+    <t>DAY 4</t>
+  </si>
+  <si>
+    <t>DAY 5</t>
+  </si>
+  <si>
+    <t>DAY 6</t>
   </si>
   <si>
     <t>3x8</t>
   </si>
   <si>
-    <t>Incline DB Press</t>
-  </si>
-  <si>
-    <t>4x8</t>
-  </si>
-  <si>
-    <t>Incline Press Machine</t>
-  </si>
-  <si>
-    <t>3x6</t>
-  </si>
-  <si>
-    <t>DAY 2</t>
-  </si>
-  <si>
-    <t>3x12</t>
-  </si>
-  <si>
-    <t>DAY 3</t>
-  </si>
-  <si>
-    <t>4x12</t>
-  </si>
-  <si>
-    <t>4x10</t>
-  </si>
-  <si>
-    <t>DAY 4</t>
-  </si>
-  <si>
-    <t>4x6</t>
+    <t>DAY 7</t>
+  </si>
+  <si>
+    <t>DAY 8</t>
+  </si>
+  <si>
+    <t>DAY 9</t>
   </si>
 </sst>
 </file>
@@ -436,7 +451,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -566,7 +581,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -586,7 +601,7 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -601,7 +616,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2"/>
     </row>
@@ -612,7 +627,7 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -622,7 +637,7 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -632,7 +647,7 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -642,7 +657,7 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -658,7 +673,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -668,7 +683,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -678,7 +693,7 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -688,11 +703,241 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="3" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="46">
     <mergeCell ref="A1:S3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:C7"/>
@@ -714,6 +959,31 @@
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>